<commit_message>
Changed and fixed John Murungi
</commit_message>
<xml_diff>
--- a/ALICE KIBUI.xlsx
+++ b/ALICE KIBUI.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ASSETFLOW-PC\Desktop\FLORENCE\CLIENTS\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="18195" windowHeight="11760" firstSheet="2" activeTab="10"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="18195" windowHeight="11760" firstSheet="10" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="FEBRUARY 21" sheetId="1" r:id="rId1"/>
@@ -19,12 +24,12 @@
     <sheet name="NOVEMBER 21" sheetId="10" r:id="rId10"/>
     <sheet name="DECEMBER" sheetId="11" r:id="rId11"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="65">
   <si>
     <t xml:space="preserve">RENT STATEMENT </t>
   </si>
@@ -217,11 +222,14 @@
   <si>
     <t>DEC</t>
   </si>
+  <si>
+    <t>PAID ON 14/12</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="#,##0.00;\-#,##0.00"/>
@@ -434,7 +442,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -469,7 +477,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1808,7 +1816,7 @@
   <dimension ref="A1:J30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1913,10 +1921,12 @@
         <f>D5+E5+F5+G5</f>
         <v>14000</v>
       </c>
-      <c r="I5" s="3"/>
+      <c r="I5" s="3">
+        <v>14000</v>
+      </c>
       <c r="J5" s="3">
         <f>H5-I5</f>
-        <v>14000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -2061,12 +2071,11 @@
         <v>14000</v>
       </c>
       <c r="I11" s="2">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <v>14000</v>
       </c>
       <c r="J11" s="2">
         <f t="shared" si="2"/>
-        <v>14000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -2151,7 +2160,7 @@
       </c>
       <c r="G16" s="18">
         <f>I11</f>
-        <v>0</v>
+        <v>14000</v>
       </c>
       <c r="H16" s="17"/>
       <c r="I16" s="17"/>
@@ -2260,13 +2269,21 @@
       <c r="I22" s="16"/>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B23" s="21"/>
+      <c r="B23" s="21" t="s">
+        <v>64</v>
+      </c>
       <c r="C23" s="17"/>
-      <c r="D23" s="17"/>
+      <c r="D23" s="17">
+        <v>12600</v>
+      </c>
       <c r="E23" s="17"/>
-      <c r="F23" s="21"/>
+      <c r="F23" s="21" t="s">
+        <v>64</v>
+      </c>
       <c r="G23" s="17"/>
-      <c r="H23" s="17"/>
+      <c r="H23" s="17">
+        <v>12600</v>
+      </c>
       <c r="I23" s="17"/>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.25">
@@ -2299,26 +2316,26 @@
       </c>
       <c r="D26" s="20">
         <f>SUM(D23:D25)</f>
-        <v>0</v>
+        <v>12600</v>
       </c>
       <c r="E26" s="20">
         <f>C26-D26</f>
-        <v>12600</v>
+        <v>0</v>
       </c>
       <c r="F26" s="16" t="s">
         <v>18</v>
       </c>
       <c r="G26" s="20">
         <f>G16+G17-H21</f>
-        <v>-1400</v>
+        <v>12600</v>
       </c>
       <c r="H26" s="20">
         <f>SUM(H23:H25)</f>
-        <v>0</v>
+        <v>12600</v>
       </c>
       <c r="I26" s="20">
         <f>G26-H26</f>
-        <v>-1400</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.25">

</xml_diff>